<commit_message>
saving module 3 work
</commit_message>
<xml_diff>
--- a/Module3/TimesheetCS5010.xlsx
+++ b/Module3/TimesheetCS5010.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doyle\Documents\GitHub\CS5010_NotesEtc\Module3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="27795" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +79,21 @@
   </si>
   <si>
     <t xml:space="preserve"> =========================committing to git: 1/28 9:16 =========================</t>
+  </si>
+  <si>
+    <t>Had to revert/redo last checkin - accidentally overwrite set01 notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 1/29 17:17 =========================</t>
+  </si>
+  <si>
+    <t>Started rectangle, constants, data-definition and initial world = static.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 1/30 18:45 =========================</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -568,7 +588,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -577,6 +597,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -628,6 +650,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -675,7 +700,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -710,7 +735,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -919,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,14 +968,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="8"/>
       <c r="K1" t="s">
         <v>7</v>
       </c>
@@ -984,11 +1009,11 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>41667</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
@@ -997,103 +1022,212 @@
       <c r="D4" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>41668</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7">
+        <v>10</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>41669</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.77916666666666667</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7">
+        <v>40</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4">
-        <f>SUMIF(G3:G7,"1",I3:I7)</f>
+      <c r="G12" s="4">
+        <f>SUMIF(G3:G11,"1",I3:I11)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="4">
+        <f>SUMIF(G3:G11,"2",I3:I11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4">
+        <f>SUMIF(G3:G11,"3",I3:I11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="4">
+        <f>SUMIF(G3:G11,"4",I3:I11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="3">
+        <f>G12/60</f>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="4">
-        <f>SUMIF(G3:G7,"2",I3:I7)</f>
+      <c r="G18" s="3">
+        <f>G13/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4">
-        <f>SUMIF(G3:G7,"3",I3:I7)</f>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3">
+        <f>G14/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4">
-        <f>SUMIF(G3:G7,"4",I3:I7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="3">
-        <f>G8/60</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="3">
-        <f>G9/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3">
-        <f>G10/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3">
-        <f>G11/60</f>
+      <c r="G20" s="3">
+        <f>G15/60</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to notes and timesheet
</commit_message>
<xml_diff>
--- a/Module3/TimesheetCS5010.xlsx
+++ b/Module3/TimesheetCS5010.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doyle\Documents\GitHub\CS5010_NotesEtc\Module3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="27795" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +89,93 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 1/31 13:40 =========================</t>
+  </si>
+  <si>
+    <t>More work on rectangle, borrowing heavily from draggable cat.   Initial goal = a "toggleable" rectangle</t>
+  </si>
+  <si>
+    <t>Moved over some tests from draggable cat, made them work for new world</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 1/31 14:35 =========================</t>
+  </si>
+  <si>
+    <t>m/dd</t>
+  </si>
+  <si>
+    <t>hh:ss</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>Got selectable/draggable working with ported tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 1/31 18:00 =========================</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: m/dd hh:ss =========================</t>
+  </si>
+  <si>
+    <t>Got centered red circle working, test coverage for all except big-bang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/1 15:28 =========================</t>
+  </si>
+  <si>
+    <t>Got solution working with mouse &lt;&gt; rect center.  Needs a bit of cleanup and tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/1 16:41 =========================</t>
+  </si>
+  <si>
+    <t>More commenting in rectangle</t>
+  </si>
+  <si>
+    <t>Copied over two draggable cats.  Added direction property to struct and the direction? Helpers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/1 18:30 =========================</t>
+  </si>
+  <si>
+    <t>Added movement handling for selected cats</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/1 22:13 =========================</t>
+  </si>
+  <si>
+    <t>got bouncing working, some work on comments and tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/2 10:50 =========================</t>
+  </si>
+  <si>
+    <t>Worked on smoother bouncing, improved test coverage</t>
+  </si>
+  <si>
+    <t>finish  arrow key tests</t>
+  </si>
+  <si>
+    <t>bounce tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/3 13:06  =========================</t>
+  </si>
+  <si>
+    <t>ensure all provided functs tests pass</t>
+  </si>
+  <si>
+    <t>Review commenting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/3 16:37  =========================</t>
   </si>
 </sst>
 </file>
@@ -588,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -598,7 +680,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -700,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,7 +816,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -944,16 +1025,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -968,20 +1052,19 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
       <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1006,11 +1089,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="2">
         <v>41667</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1039,7 +1119,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="7"/>
@@ -1054,7 +1134,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="2">
         <v>41668</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1083,7 +1163,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="7"/>
@@ -1098,7 +1178,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="2">
         <v>41669</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1127,7 +1207,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="7"/>
@@ -1141,101 +1221,629 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>41670</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>45</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41670</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>15</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>41670</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8">
+        <f>60+50</f>
+        <v>110</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5805555555555556</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.6430555555555556</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8">
+        <f>60+26</f>
+        <v>86</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8">
+        <v>60</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.71666666666666667</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8">
+        <f>15+12</f>
+        <v>27</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.76944444444444438</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>2</v>
+      </c>
+      <c r="I21" s="8">
+        <f>45+28</f>
+        <v>73</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.89513888888888893</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.9243055555555556</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>2</v>
+      </c>
+      <c r="I23" s="8">
+        <f>31+11</f>
+        <v>42</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>41672</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.45069444444444445</v>
+      </c>
+      <c r="E25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>2</v>
+      </c>
+      <c r="I25" s="8">
+        <f>45+60+30</f>
+        <v>135</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E27" s="8">
+        <v>2</v>
+      </c>
+      <c r="G27" s="8">
+        <v>2</v>
+      </c>
+      <c r="I27" s="8">
+        <f>15+60+40</f>
+        <v>115</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8">
+        <v>2</v>
+      </c>
+      <c r="I28" s="8">
+        <v>15</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="E29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>2</v>
+      </c>
+      <c r="I29" s="8">
+        <f>60+25</f>
+        <v>85</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <v>2</v>
+      </c>
+      <c r="I31" s="8">
+        <v>7</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8">
+        <v>3</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+      <c r="G33" s="8">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <v>22</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+      <c r="G34" s="8">
+        <v>2</v>
+      </c>
+      <c r="I34" s="8">
+        <f>32+16</f>
+        <v>48</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>41673</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.69166666666666676</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
+      <c r="I35" s="8">
+        <f>36-16</f>
+        <v>20</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="39" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="4">
-        <f>SUMIF(G3:G11,"1",I3:I11)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="G39" s="4">
+        <f>SUMIF(G3:G38,"1",I3:I38)</f>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="4">
-        <f>SUMIF(G3:G11,"2",I3:I11)</f>
+      <c r="G40" s="4">
+        <f>SUMIF(G3:G38,"2",I3:I38)</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4">
+        <f>SUMIF(G3:G38,"3",I3:I38)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="4">
-        <f>SUMIF(G3:G11,"3",I3:I11)</f>
+    <row r="42" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="4">
+        <f>SUMIF(G3:G38,"4",I3:I38)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="4">
-        <f>SUMIF(G3:G11,"4",I3:I11)</f>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="3">
+        <f>G39/60</f>
+        <v>7.3833333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="3">
+        <f>G40/60</f>
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="3">
+        <f>G41/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="3">
-        <f>G12/60</f>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="3">
-        <f>G13/60</f>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="3">
+        <f>G42/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="3">
-        <f>G14/60</f>
+    <row r="52" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="3">
-        <f>G15/60</f>
-        <v>0</v>
+      <c r="G52" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>